<commit_message>
modified file added new Baseclass lib
</commit_message>
<xml_diff>
--- a/SDET/testData/testScriptData.xlsx
+++ b/SDET/testData/testScriptData.xlsx
@@ -3,20 +3,16 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SR Studio\Desktop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF5A6A7E-7FC7-4506-9E09-C52E3151AE92}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{F5FE5418-1249-4DEE-84B1-CA95513715FA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2304" yWindow="2304" windowWidth="23280" windowHeight="13224" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="org" sheetId="1" r:id="rId1"/>
     <sheet name="contact" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1:F12"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -413,8 +409,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -502,8 +498,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB901F64-B97D-4099-B7B0-E50AA34C6726}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>